<commit_message>
final working wsbot for images and text
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -438,42 +438,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Camí jeancon</t>
+          <t>bien supongo</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bautista maldonafo</t>
+          <t>ajjasjassj</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bauti castellano</t>
+          <t>Es muy</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mati passanisi</t>
+          <t>lindo</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mateo stibel</t>
+          <t>todo bien</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tomas dominguez</t>
+          <t>vos</t>
         </is>
       </c>
     </row>

</xml_diff>